<commit_message>
wrapped up leetcode for the day. 2 easies and a medium on the array-string topic.
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vt653f\Documents\Python\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE0A575-096B-46BA-A731-5E0F348B7159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B6DF75-3FAF-4674-92C8-C4EDD6A4CE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19305" yWindow="0" windowWidth="9810" windowHeight="14745" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>Begin Leetcode Top Interview 150?</t>
+  </si>
+  <si>
+    <t>151, 1071, 1768</t>
+  </si>
+  <si>
+    <t>High</t>
   </si>
 </sst>
 </file>
@@ -169,7 +175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,6 +200,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -207,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -215,13 +227,16 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -561,7 +576,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -574,27 +589,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="6">
         <v>45973</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -605,6 +620,12 @@
       </c>
       <c r="D2" s="1">
         <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -639,13 +660,13 @@
       <c r="A5" s="2">
         <v>45976</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -749,13 +770,13 @@
       <c r="A13" s="2">
         <v>45983</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -845,13 +866,13 @@
       <c r="A20" s="2">
         <v>45990</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
@@ -941,13 +962,13 @@
       <c r="A27" s="2">
         <v>45997</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
@@ -1037,13 +1058,13 @@
       <c r="A34" s="2">
         <v>46004</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
@@ -1133,13 +1154,13 @@
       <c r="A41" s="2">
         <v>46011</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
@@ -1302,22 +1323,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1511,13 +1532,13 @@
       <c r="A18" s="2">
         <v>45674</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -1607,13 +1628,13 @@
       <c r="A25" s="2">
         <v>45681</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
@@ -1670,13 +1691,13 @@
       <c r="A32" s="2">
         <v>45688</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">

</xml_diff>

<commit_message>
wrapped up the daily.
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vt653f\Documents\Python\Leetcode_Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B6DF75-3FAF-4674-92C8-C4EDD6A4CE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869B2811-737C-45D7-A9CC-FBBE1EF12BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
+    <workbookView xWindow="-38490" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -21,23 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -154,6 +143,9 @@
   </si>
   <si>
     <t>High</t>
+  </si>
+  <si>
+    <t>1431, 605, 238</t>
   </si>
 </sst>
 </file>
@@ -230,13 +222,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -576,19 +568,19 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="30.7109375" style="1"/>
+    <col min="3" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="30.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -608,8 +600,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
         <v>45973</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -628,7 +620,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>45974</v>
       </c>
@@ -641,8 +633,11 @@
       <c r="D3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>45975</v>
       </c>
@@ -656,19 +651,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>45976</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>45977</v>
       </c>
@@ -682,7 +677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>45978</v>
       </c>
@@ -696,7 +691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45979</v>
       </c>
@@ -710,7 +705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>45980</v>
       </c>
@@ -724,7 +719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>45981</v>
       </c>
@@ -738,7 +733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>45981</v>
       </c>
@@ -752,7 +747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>45982</v>
       </c>
@@ -766,19 +761,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>45983</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>45984</v>
       </c>
@@ -792,7 +787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>45985</v>
       </c>
@@ -806,7 +801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>45986</v>
       </c>
@@ -820,7 +815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>45987</v>
       </c>
@@ -834,7 +829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>45988</v>
       </c>
@@ -848,7 +843,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>45989</v>
       </c>
@@ -862,19 +857,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>45990</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>45991</v>
       </c>
@@ -888,7 +883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>45992</v>
       </c>
@@ -902,7 +897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>45993</v>
       </c>
@@ -916,7 +911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>45994</v>
       </c>
@@ -930,7 +925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>45995</v>
       </c>
@@ -944,7 +939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>45996</v>
       </c>
@@ -958,19 +953,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>45997</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-    </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>45998</v>
       </c>
@@ -984,7 +979,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>45999</v>
       </c>
@@ -998,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>46000</v>
       </c>
@@ -1012,7 +1007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>46001</v>
       </c>
@@ -1026,7 +1021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>46002</v>
       </c>
@@ -1040,7 +1035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>46003</v>
       </c>
@@ -1054,19 +1049,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>46004</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-    </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>46005</v>
       </c>
@@ -1080,7 +1075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>46006</v>
       </c>
@@ -1094,7 +1089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>46007</v>
       </c>
@@ -1108,7 +1103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>46008</v>
       </c>
@@ -1122,7 +1117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>46009</v>
       </c>
@@ -1136,7 +1131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>46010</v>
       </c>
@@ -1150,19 +1145,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>46011</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-    </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>46012</v>
       </c>
@@ -1176,7 +1171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>46013</v>
       </c>
@@ -1190,7 +1185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>46014</v>
       </c>
@@ -1204,7 +1199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>46015</v>
       </c>
@@ -1218,77 +1213,77 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>46016</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-    </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+    </row>
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>46017</v>
       </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-    </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+    </row>
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>46018</v>
       </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-    </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+    </row>
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>46019</v>
       </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-    </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+    </row>
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>46020</v>
       </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-    </row>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+    </row>
+    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>46021</v>
       </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-    </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+    </row>
+    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>46022</v>
       </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1313,16 +1308,16 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="1"/>
+    <col min="1" max="1" width="30.7265625" style="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="30.7109375" style="1"/>
+    <col min="3" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="30.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1342,109 +1337,109 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>45658</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>45659</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>45660</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>45661</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>45662</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>45663</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45664</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>45665</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>45666</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>45667</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>45668</v>
       </c>
@@ -1458,7 +1453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>45669</v>
       </c>
@@ -1472,7 +1467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>45670</v>
       </c>
@@ -1486,7 +1481,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>45671</v>
       </c>
@@ -1500,7 +1495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>45672</v>
       </c>
@@ -1514,7 +1509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>45673</v>
       </c>
@@ -1528,19 +1523,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>45674</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>45675</v>
       </c>
@@ -1554,7 +1549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>45676</v>
       </c>
@@ -1568,7 +1563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>45677</v>
       </c>
@@ -1582,7 +1577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>45678</v>
       </c>
@@ -1596,7 +1591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>45679</v>
       </c>
@@ -1610,7 +1605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>45680</v>
       </c>
@@ -1624,19 +1619,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>45681</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-    </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>45682</v>
       </c>
@@ -1650,7 +1645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>45683</v>
       </c>
@@ -1664,7 +1659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>45684</v>
       </c>
@@ -1672,34 +1667,34 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>45685</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>45686</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>45687</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>45688</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>45689</v>
       </c>

</xml_diff>

<commit_message>
dailys done for the day. 1 easy and two medium Array/string questions
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869B2811-737C-45D7-A9CC-FBBE1EF12BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C6E085-864F-46E1-BEC8-438CC2E5B392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38490" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
   <si>
     <t>Date</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>1431, 605, 238</t>
+  </si>
+  <si>
+    <t>Add in Maps</t>
+  </si>
+  <si>
+    <t>345, 334, 443</t>
   </si>
 </sst>
 </file>
@@ -568,7 +574,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -636,6 +642,9 @@
       <c r="E3" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
@@ -649,6 +658,9 @@
       </c>
       <c r="D4" s="1">
         <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1305,7 +1317,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1671,6 +1683,9 @@
       <c r="A29" s="2">
         <v>45685</v>
       </c>
+      <c r="B29" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2">

</xml_diff>

<commit_message>
setup medium two pointer for tomorrow
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C6E085-864F-46E1-BEC8-438CC2E5B392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BECCBC-F921-4F42-949D-1EF8A826D687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38490" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
+    <workbookView xWindow="-35760" yWindow="3920" windowWidth="28800" windowHeight="15370" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -574,7 +574,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -687,6 +687,9 @@
       </c>
       <c r="D6" s="1">
         <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Dailies for two pointer algorithm. Done with two pointer after today.
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vt653f\Documents\Python\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BECCBC-F921-4F42-949D-1EF8A826D687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE9043D-08C3-4A0A-8507-C130C7E22DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35760" yWindow="3920" windowWidth="28800" windowHeight="15370" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -152,6 +152,15 @@
   </si>
   <si>
     <t>345, 334, 443</t>
+  </si>
+  <si>
+    <t>283, 11</t>
+  </si>
+  <si>
+    <t>Note: two pointers can start from either end. Both beginning, or opposite ends</t>
+  </si>
+  <si>
+    <t>392, 1679</t>
   </si>
 </sst>
 </file>
@@ -574,19 +583,21 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="30.7265625" style="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.42578125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="30.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -606,7 +617,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>45973</v>
       </c>
@@ -626,7 +637,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45974</v>
       </c>
@@ -646,7 +657,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45975</v>
       </c>
@@ -663,7 +674,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45976</v>
       </c>
@@ -675,7 +686,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45977</v>
       </c>
@@ -688,11 +699,14 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="1">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45978</v>
       </c>
@@ -705,8 +719,14 @@
       <c r="D7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45979</v>
       </c>
@@ -720,7 +740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45980</v>
       </c>
@@ -734,7 +754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45981</v>
       </c>
@@ -748,7 +768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45981</v>
       </c>
@@ -762,7 +782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45982</v>
       </c>
@@ -776,7 +796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45983</v>
       </c>
@@ -788,7 +808,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45984</v>
       </c>
@@ -802,7 +822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45985</v>
       </c>
@@ -816,7 +836,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45986</v>
       </c>
@@ -830,7 +850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45987</v>
       </c>
@@ -844,7 +864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45988</v>
       </c>
@@ -858,7 +878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45989</v>
       </c>
@@ -872,7 +892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45990</v>
       </c>
@@ -884,7 +904,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45991</v>
       </c>
@@ -898,7 +918,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45992</v>
       </c>
@@ -912,7 +932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45993</v>
       </c>
@@ -926,7 +946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45994</v>
       </c>
@@ -940,7 +960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45995</v>
       </c>
@@ -954,7 +974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45996</v>
       </c>
@@ -968,7 +988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45997</v>
       </c>
@@ -980,7 +1000,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>45998</v>
       </c>
@@ -994,7 +1014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>45999</v>
       </c>
@@ -1008,7 +1028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>46000</v>
       </c>
@@ -1022,7 +1042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>46001</v>
       </c>
@@ -1036,7 +1056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>46002</v>
       </c>
@@ -1050,7 +1070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>46003</v>
       </c>
@@ -1064,7 +1084,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>46004</v>
       </c>
@@ -1076,7 +1096,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>46005</v>
       </c>
@@ -1090,7 +1110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>46006</v>
       </c>
@@ -1104,7 +1124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>46007</v>
       </c>
@@ -1118,7 +1138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>46008</v>
       </c>
@@ -1132,7 +1152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>46009</v>
       </c>
@@ -1146,7 +1166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>46010</v>
       </c>
@@ -1160,7 +1180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>46011</v>
       </c>
@@ -1172,7 +1192,7 @@
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>46012</v>
       </c>
@@ -1186,7 +1206,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>46013</v>
       </c>
@@ -1200,7 +1220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>46014</v>
       </c>
@@ -1214,7 +1234,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>46015</v>
       </c>
@@ -1228,7 +1248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>46016</v>
       </c>
@@ -1240,7 +1260,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46017</v>
       </c>
@@ -1250,7 +1270,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>46018</v>
       </c>
@@ -1260,7 +1280,7 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>46019</v>
       </c>
@@ -1270,7 +1290,7 @@
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>46020</v>
       </c>
@@ -1280,7 +1300,7 @@
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>46021</v>
       </c>
@@ -1290,7 +1310,7 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
     </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>46022</v>
       </c>
@@ -1323,16 +1343,16 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7265625" style="1"/>
+    <col min="1" max="1" width="30.7109375" style="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="30.7265625" style="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="30.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1352,7 +1372,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45658</v>
       </c>
@@ -1364,7 +1384,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45659</v>
       </c>
@@ -1374,7 +1394,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45660</v>
       </c>
@@ -1384,7 +1404,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45661</v>
       </c>
@@ -1394,7 +1414,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45662</v>
       </c>
@@ -1404,7 +1424,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45663</v>
       </c>
@@ -1414,7 +1434,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45664</v>
       </c>
@@ -1424,7 +1444,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45665</v>
       </c>
@@ -1434,7 +1454,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45666</v>
       </c>
@@ -1444,7 +1464,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45667</v>
       </c>
@@ -1454,7 +1474,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45668</v>
       </c>
@@ -1468,7 +1488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45669</v>
       </c>
@@ -1482,7 +1502,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45670</v>
       </c>
@@ -1496,7 +1516,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45671</v>
       </c>
@@ -1510,7 +1530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45672</v>
       </c>
@@ -1524,7 +1544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45673</v>
       </c>
@@ -1538,7 +1558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45674</v>
       </c>
@@ -1550,7 +1570,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45675</v>
       </c>
@@ -1564,7 +1584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45676</v>
       </c>
@@ -1578,7 +1598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45677</v>
       </c>
@@ -1592,7 +1612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45678</v>
       </c>
@@ -1606,7 +1626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45679</v>
       </c>
@@ -1620,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45680</v>
       </c>
@@ -1634,7 +1654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45681</v>
       </c>
@@ -1646,7 +1666,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45682</v>
       </c>
@@ -1660,7 +1680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45683</v>
       </c>
@@ -1674,7 +1694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>45684</v>
       </c>
@@ -1682,7 +1702,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>45685</v>
       </c>
@@ -1690,17 +1710,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>45686</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>45687</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>45688</v>
       </c>
@@ -1712,7 +1732,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>45689</v>
       </c>

</xml_diff>

<commit_message>
Dailys for sliding window, I may come back to this one. I can do it, but it get turned around here and there.
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vt653f\Documents\Python\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE9043D-08C3-4A0A-8507-C130C7E22DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B647186-023A-4B50-851F-50287189A412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
+    <workbookView xWindow="-16305" yWindow="0" windowWidth="14400" windowHeight="10755" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>392, 1679</t>
+  </si>
+  <si>
+    <t>643, 1456</t>
+  </si>
+  <si>
+    <t>Med</t>
   </si>
 </sst>
 </file>
@@ -583,7 +589,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -738,6 +744,12 @@
       </c>
       <c r="D8" s="1">
         <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
need to do another tomorrow.
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vt653f\Documents\Python\Leetcode_Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B647186-023A-4B50-851F-50287189A412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315EB8EA-CB4A-41E4-A2CB-85DDA97AA423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16305" yWindow="0" windowWidth="14400" windowHeight="10755" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
+    <workbookView xWindow="-38490" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>Med</t>
+  </si>
+  <si>
+    <t>1004, 1493</t>
   </si>
 </sst>
 </file>
@@ -588,22 +591,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B13EEB8-513E-4F27-BA22-1B05F2BB10E7}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.42578125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="30.7109375" style="1"/>
+    <col min="3" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.453125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="30.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -623,7 +626,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>45973</v>
       </c>
@@ -643,7 +646,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>45974</v>
       </c>
@@ -663,7 +666,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>45975</v>
       </c>
@@ -680,7 +683,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>45976</v>
       </c>
@@ -692,7 +695,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>45977</v>
       </c>
@@ -712,7 +715,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>45978</v>
       </c>
@@ -732,7 +735,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45979</v>
       </c>
@@ -752,7 +755,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>45980</v>
       </c>
@@ -765,8 +768,14 @@
       <c r="D9" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>45981</v>
       </c>
@@ -780,7 +789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>45981</v>
       </c>
@@ -794,7 +803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>45982</v>
       </c>
@@ -808,7 +817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>45983</v>
       </c>
@@ -820,7 +829,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>45984</v>
       </c>
@@ -834,7 +843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>45985</v>
       </c>
@@ -848,7 +857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>45986</v>
       </c>
@@ -862,7 +871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>45987</v>
       </c>
@@ -876,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>45988</v>
       </c>
@@ -890,7 +899,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>45989</v>
       </c>
@@ -904,7 +913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>45990</v>
       </c>
@@ -916,7 +925,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>45991</v>
       </c>
@@ -930,7 +939,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>45992</v>
       </c>
@@ -944,7 +953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>45993</v>
       </c>
@@ -958,7 +967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>45994</v>
       </c>
@@ -972,7 +981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>45995</v>
       </c>
@@ -986,7 +995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>45996</v>
       </c>
@@ -1000,7 +1009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>45997</v>
       </c>
@@ -1012,7 +1021,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>45998</v>
       </c>
@@ -1026,7 +1035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>45999</v>
       </c>
@@ -1040,7 +1049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>46000</v>
       </c>
@@ -1054,7 +1063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>46001</v>
       </c>
@@ -1068,7 +1077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>46002</v>
       </c>
@@ -1082,7 +1091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>46003</v>
       </c>
@@ -1096,7 +1105,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>46004</v>
       </c>
@@ -1108,7 +1117,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>46005</v>
       </c>
@@ -1122,7 +1131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>46006</v>
       </c>
@@ -1136,7 +1145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>46007</v>
       </c>
@@ -1150,7 +1159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>46008</v>
       </c>
@@ -1164,7 +1173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>46009</v>
       </c>
@@ -1178,7 +1187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>46010</v>
       </c>
@@ -1192,7 +1201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>46011</v>
       </c>
@@ -1204,7 +1213,7 @@
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>46012</v>
       </c>
@@ -1218,7 +1227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>46013</v>
       </c>
@@ -1232,7 +1241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>46014</v>
       </c>
@@ -1246,7 +1255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>46015</v>
       </c>
@@ -1260,7 +1269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>46016</v>
       </c>
@@ -1272,7 +1281,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>46017</v>
       </c>
@@ -1282,7 +1291,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>46018</v>
       </c>
@@ -1292,7 +1301,7 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>46019</v>
       </c>
@@ -1302,7 +1311,7 @@
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>46020</v>
       </c>
@@ -1312,7 +1321,7 @@
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>46021</v>
       </c>
@@ -1322,7 +1331,7 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
     </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>46022</v>
       </c>
@@ -1355,16 +1364,16 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="1"/>
+    <col min="1" max="1" width="30.7265625" style="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="30.7109375" style="1"/>
+    <col min="3" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="30.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1384,7 +1393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>45658</v>
       </c>
@@ -1396,7 +1405,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>45659</v>
       </c>
@@ -1406,7 +1415,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>45660</v>
       </c>
@@ -1416,7 +1425,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>45661</v>
       </c>
@@ -1426,7 +1435,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>45662</v>
       </c>
@@ -1436,7 +1445,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>45663</v>
       </c>
@@ -1446,7 +1455,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45664</v>
       </c>
@@ -1456,7 +1465,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>45665</v>
       </c>
@@ -1466,7 +1475,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>45666</v>
       </c>
@@ -1476,7 +1485,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>45667</v>
       </c>
@@ -1486,7 +1495,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>45668</v>
       </c>
@@ -1500,7 +1509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>45669</v>
       </c>
@@ -1514,7 +1523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>45670</v>
       </c>
@@ -1528,7 +1537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>45671</v>
       </c>
@@ -1542,7 +1551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>45672</v>
       </c>
@@ -1556,7 +1565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>45673</v>
       </c>
@@ -1570,7 +1579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>45674</v>
       </c>
@@ -1582,7 +1591,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>45675</v>
       </c>
@@ -1596,7 +1605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>45676</v>
       </c>
@@ -1610,7 +1619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>45677</v>
       </c>
@@ -1624,7 +1633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>45678</v>
       </c>
@@ -1638,7 +1647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>45679</v>
       </c>
@@ -1652,7 +1661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>45680</v>
       </c>
@@ -1666,7 +1675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>45681</v>
       </c>
@@ -1678,7 +1687,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>45682</v>
       </c>
@@ -1692,7 +1701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>45683</v>
       </c>
@@ -1706,7 +1715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>45684</v>
       </c>
@@ -1714,7 +1723,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>45685</v>
       </c>
@@ -1722,17 +1731,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>45686</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>45687</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>45688</v>
       </c>
@@ -1744,7 +1753,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>45689</v>
       </c>

</xml_diff>

<commit_message>
two done. The rest outlined
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315EB8EA-CB4A-41E4-A2CB-85DDA97AA423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B21F91D-582B-483A-84FC-E4E6065198AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38490" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>1004, 1493</t>
+  </si>
+  <si>
+    <t>724, 1732</t>
   </si>
 </sst>
 </file>
@@ -591,22 +594,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B13EEB8-513E-4F27-BA22-1B05F2BB10E7}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="30.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="1" customWidth="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.453125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="30.7265625" style="1"/>
+    <col min="3" max="3" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.44140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="30.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -626,7 +629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>45973</v>
       </c>
@@ -646,7 +649,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45974</v>
       </c>
@@ -666,7 +669,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>45975</v>
       </c>
@@ -683,7 +686,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>45976</v>
       </c>
@@ -695,7 +698,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>45977</v>
       </c>
@@ -715,7 +718,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45978</v>
       </c>
@@ -735,7 +738,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>45979</v>
       </c>
@@ -755,7 +758,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>45980</v>
       </c>
@@ -775,7 +778,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>45981</v>
       </c>
@@ -788,8 +791,14 @@
       <c r="D10" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>45981</v>
       </c>
@@ -803,7 +812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>45982</v>
       </c>
@@ -817,7 +826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>45983</v>
       </c>
@@ -829,7 +838,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>45984</v>
       </c>
@@ -843,7 +852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>45985</v>
       </c>
@@ -857,7 +866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>45986</v>
       </c>
@@ -871,7 +880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>45987</v>
       </c>
@@ -885,7 +894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>45988</v>
       </c>
@@ -899,7 +908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>45989</v>
       </c>
@@ -913,7 +922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>45990</v>
       </c>
@@ -925,7 +934,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>45991</v>
       </c>
@@ -939,7 +948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>45992</v>
       </c>
@@ -953,7 +962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>45993</v>
       </c>
@@ -967,7 +976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>45994</v>
       </c>
@@ -981,7 +990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>45995</v>
       </c>
@@ -995,7 +1004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>45996</v>
       </c>
@@ -1009,7 +1018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>45997</v>
       </c>
@@ -1021,7 +1030,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>45998</v>
       </c>
@@ -1035,7 +1044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>45999</v>
       </c>
@@ -1049,7 +1058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>46000</v>
       </c>
@@ -1063,7 +1072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>46001</v>
       </c>
@@ -1077,7 +1086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>46002</v>
       </c>
@@ -1091,7 +1100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>46003</v>
       </c>
@@ -1105,7 +1114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>46004</v>
       </c>
@@ -1117,7 +1126,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>46005</v>
       </c>
@@ -1131,7 +1140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>46006</v>
       </c>
@@ -1145,7 +1154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>46007</v>
       </c>
@@ -1159,7 +1168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>46008</v>
       </c>
@@ -1173,7 +1182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>46009</v>
       </c>
@@ -1187,7 +1196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>46010</v>
       </c>
@@ -1201,7 +1210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>46011</v>
       </c>
@@ -1213,7 +1222,7 @@
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>46012</v>
       </c>
@@ -1227,7 +1236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>46013</v>
       </c>
@@ -1241,7 +1250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>46014</v>
       </c>
@@ -1255,7 +1264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>46015</v>
       </c>
@@ -1269,7 +1278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>46016</v>
       </c>
@@ -1281,7 +1290,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46017</v>
       </c>
@@ -1291,7 +1300,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>46018</v>
       </c>
@@ -1301,7 +1310,7 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>46019</v>
       </c>
@@ -1311,7 +1320,7 @@
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>46020</v>
       </c>
@@ -1321,7 +1330,7 @@
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>46021</v>
       </c>
@@ -1331,7 +1340,7 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
     </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>46022</v>
       </c>
@@ -1364,16 +1373,16 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="30.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.7265625" style="1"/>
+    <col min="1" max="1" width="30.77734375" style="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="30.7265625" style="1"/>
+    <col min="3" max="3" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="30.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1393,7 +1402,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45658</v>
       </c>
@@ -1405,7 +1414,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45659</v>
       </c>
@@ -1415,7 +1424,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>45660</v>
       </c>
@@ -1425,7 +1434,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>45661</v>
       </c>
@@ -1435,7 +1444,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>45662</v>
       </c>
@@ -1445,7 +1454,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45663</v>
       </c>
@@ -1455,7 +1464,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>45664</v>
       </c>
@@ -1465,7 +1474,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>45665</v>
       </c>
@@ -1475,7 +1484,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>45666</v>
       </c>
@@ -1485,7 +1494,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>45667</v>
       </c>
@@ -1495,7 +1504,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>45668</v>
       </c>
@@ -1509,7 +1518,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>45669</v>
       </c>
@@ -1523,7 +1532,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>45670</v>
       </c>
@@ -1537,7 +1546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>45671</v>
       </c>
@@ -1551,7 +1560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>45672</v>
       </c>
@@ -1565,7 +1574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>45673</v>
       </c>
@@ -1579,7 +1588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>45674</v>
       </c>
@@ -1591,7 +1600,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>45675</v>
       </c>
@@ -1605,7 +1614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>45676</v>
       </c>
@@ -1619,7 +1628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>45677</v>
       </c>
@@ -1633,7 +1642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>45678</v>
       </c>
@@ -1647,7 +1656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>45679</v>
       </c>
@@ -1661,7 +1670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>45680</v>
       </c>
@@ -1675,7 +1684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>45681</v>
       </c>
@@ -1687,7 +1696,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>45682</v>
       </c>
@@ -1701,7 +1710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>45683</v>
       </c>
@@ -1715,7 +1724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>45684</v>
       </c>
@@ -1723,7 +1732,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>45685</v>
       </c>
@@ -1731,17 +1740,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>45686</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>45687</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>45688</v>
       </c>
@@ -1753,7 +1762,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>45689</v>
       </c>

</xml_diff>

<commit_message>
catching up from the travel weekend.
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B21F91D-582B-483A-84FC-E4E6065198AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E96918-8707-499C-AA5F-E9AE99DE4213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="50">
   <si>
     <t>Date</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>724, 1732</t>
+  </si>
+  <si>
+    <t>2215, 1657</t>
   </si>
 </sst>
 </file>
@@ -594,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B13EEB8-513E-4F27-BA22-1B05F2BB10E7}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -810,6 +813,9 @@
       </c>
       <c r="D11" s="1">
         <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1369,7 +1375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED83FE41-D01E-4F17-A252-9750FA2AA3E0}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
catching up on hashmaps sitting in the airport.
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E96918-8707-499C-AA5F-E9AE99DE4213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEE1200-A067-4A6B-9B15-2AEBCA22C3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="50">
   <si>
     <t>Date</t>
   </si>
@@ -598,7 +598,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -817,6 +817,9 @@
       <c r="E11" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="F11" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
@@ -830,6 +833,9 @@
       </c>
       <c r="D12" s="1">
         <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1207</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
working on time limit for 2390. Works, just not efficient enough just yet
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vt653f\Documents\Python\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEE1200-A067-4A6B-9B15-2AEBCA22C3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48502E9-E161-482C-824C-7BFD187498F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
+    <workbookView xWindow="12" yWindow="12" windowWidth="23016" windowHeight="12216" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>2215, 1657</t>
+  </si>
+  <si>
+    <t>1207, 2352</t>
   </si>
 </sst>
 </file>
@@ -598,21 +601,21 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="30.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.44140625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="30.77734375" style="1"/>
+    <col min="3" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.453125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="30.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -632,7 +635,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>45973</v>
       </c>
@@ -652,7 +655,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>45974</v>
       </c>
@@ -672,7 +675,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>45975</v>
       </c>
@@ -689,7 +692,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>45976</v>
       </c>
@@ -701,7 +704,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>45977</v>
       </c>
@@ -721,7 +724,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>45978</v>
       </c>
@@ -741,7 +744,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45979</v>
       </c>
@@ -761,7 +764,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>45980</v>
       </c>
@@ -781,7 +784,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>45981</v>
       </c>
@@ -801,7 +804,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>45981</v>
       </c>
@@ -821,7 +824,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>45982</v>
       </c>
@@ -834,11 +837,14 @@
       <c r="D12" s="1">
         <v>1</v>
       </c>
-      <c r="E12" s="1">
-        <v>1207</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>45983</v>
       </c>
@@ -850,7 +856,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>45984</v>
       </c>
@@ -864,7 +870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>45985</v>
       </c>
@@ -878,7 +884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>45986</v>
       </c>
@@ -892,7 +898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>45987</v>
       </c>
@@ -906,7 +912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>45988</v>
       </c>
@@ -920,7 +926,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>45989</v>
       </c>
@@ -934,7 +940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>45990</v>
       </c>
@@ -946,7 +952,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>45991</v>
       </c>
@@ -960,7 +966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>45992</v>
       </c>
@@ -974,7 +980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>45993</v>
       </c>
@@ -988,7 +994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>45994</v>
       </c>
@@ -1002,7 +1008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>45995</v>
       </c>
@@ -1016,7 +1022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>45996</v>
       </c>
@@ -1030,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>45997</v>
       </c>
@@ -1042,7 +1048,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>45998</v>
       </c>
@@ -1056,7 +1062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>45999</v>
       </c>
@@ -1070,7 +1076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>46000</v>
       </c>
@@ -1084,7 +1090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>46001</v>
       </c>
@@ -1098,7 +1104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>46002</v>
       </c>
@@ -1112,7 +1118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>46003</v>
       </c>
@@ -1126,7 +1132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>46004</v>
       </c>
@@ -1138,7 +1144,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>46005</v>
       </c>
@@ -1152,7 +1158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>46006</v>
       </c>
@@ -1166,7 +1172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>46007</v>
       </c>
@@ -1180,7 +1186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>46008</v>
       </c>
@@ -1194,7 +1200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>46009</v>
       </c>
@@ -1208,7 +1214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>46010</v>
       </c>
@@ -1222,7 +1228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>46011</v>
       </c>
@@ -1234,7 +1240,7 @@
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>46012</v>
       </c>
@@ -1248,7 +1254,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>46013</v>
       </c>
@@ -1262,7 +1268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>46014</v>
       </c>
@@ -1276,7 +1282,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>46015</v>
       </c>
@@ -1290,7 +1296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>46016</v>
       </c>
@@ -1302,7 +1308,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>46017</v>
       </c>
@@ -1312,7 +1318,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>46018</v>
       </c>
@@ -1322,7 +1328,7 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>46019</v>
       </c>
@@ -1332,7 +1338,7 @@
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>46020</v>
       </c>
@@ -1342,7 +1348,7 @@
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>46021</v>
       </c>
@@ -1352,7 +1358,7 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
     </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>46022</v>
       </c>
@@ -1385,16 +1391,16 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="30.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.77734375" style="1"/>
+    <col min="1" max="1" width="30.81640625" style="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="30.77734375" style="1"/>
+    <col min="3" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="30.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1414,7 +1420,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>45658</v>
       </c>
@@ -1426,7 +1432,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>45659</v>
       </c>
@@ -1436,7 +1442,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>45660</v>
       </c>
@@ -1446,7 +1452,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>45661</v>
       </c>
@@ -1456,7 +1462,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>45662</v>
       </c>
@@ -1466,7 +1472,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>45663</v>
       </c>
@@ -1476,7 +1482,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45664</v>
       </c>
@@ -1486,7 +1492,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>45665</v>
       </c>
@@ -1496,7 +1502,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>45666</v>
       </c>
@@ -1506,7 +1512,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>45667</v>
       </c>
@@ -1516,7 +1522,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>45668</v>
       </c>
@@ -1530,7 +1536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>45669</v>
       </c>
@@ -1544,7 +1550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>45670</v>
       </c>
@@ -1558,7 +1564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>45671</v>
       </c>
@@ -1572,7 +1578,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>45672</v>
       </c>
@@ -1586,7 +1592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>45673</v>
       </c>
@@ -1600,7 +1606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>45674</v>
       </c>
@@ -1612,7 +1618,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>45675</v>
       </c>
@@ -1626,7 +1632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>45676</v>
       </c>
@@ -1640,7 +1646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>45677</v>
       </c>
@@ -1654,7 +1660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>45678</v>
       </c>
@@ -1668,7 +1674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>45679</v>
       </c>
@@ -1682,7 +1688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>45680</v>
       </c>
@@ -1696,7 +1702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>45681</v>
       </c>
@@ -1708,7 +1714,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>45682</v>
       </c>
@@ -1722,7 +1728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>45683</v>
       </c>
@@ -1736,7 +1742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>45684</v>
       </c>
@@ -1744,7 +1750,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>45685</v>
       </c>
@@ -1752,17 +1758,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>45686</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>45687</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>45688</v>
       </c>
@@ -1774,7 +1780,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>45689</v>
       </c>

</xml_diff>

<commit_message>
I'll do this tomorrow. Need to do 2390 and 844
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vt653f\Documents\Python\Leetcode_Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48502E9-E161-482C-824C-7BFD187498F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0FD33C-F6F3-41DE-B277-4D758DFB7BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12" yWindow="12" windowWidth="23016" windowHeight="12216" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
+    <workbookView xWindow="4970" yWindow="1930" windowWidth="28800" windowHeight="15370" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>1207, 2352</t>
+  </si>
+  <si>
+    <t>2390, 844, 1047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to do the last two. </t>
   </si>
 </sst>
 </file>
@@ -601,7 +607,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -868,6 +874,12 @@
       </c>
       <c r="D14" s="1">
         <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
still catching up from the weekend.
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vt653f\Documents\Python\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0FD33C-F6F3-41DE-B277-4D758DFB7BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594DA78E-157E-419F-9861-62024C71DE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4970" yWindow="1930" windowWidth="28800" windowHeight="15370" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -181,10 +181,10 @@
     <t>1207, 2352</t>
   </si>
   <si>
-    <t>2390, 844, 1047</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Need to do the last two. </t>
+    <t>2390, 844, 1047, 1598</t>
+  </si>
+  <si>
+    <t>Med-High</t>
   </si>
 </sst>
 </file>
@@ -606,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B13EEB8-513E-4F27-BA22-1B05F2BB10E7}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
need to finish 394 and 735 still.
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vt653f\Documents\Python\Leetcode_Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594DA78E-157E-419F-9861-62024C71DE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE875D8-754C-4EB3-A93B-8069635B2A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>Med-High</t>
+  </si>
+  <si>
+    <t>394, 735, 225, 496</t>
+  </si>
+  <si>
+    <t>need to do 394 and 735 yet</t>
   </si>
 </sst>
 </file>
@@ -607,7 +613,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -616,7 +622,7 @@
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.26953125" style="1" customWidth="1"/>
     <col min="6" max="6" width="69.453125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="30.81640625" style="1"/>
   </cols>
@@ -894,6 +900,12 @@
       </c>
       <c r="D15" s="1">
         <v>2</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
done with stacks, moving on to queues
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE875D8-754C-4EB3-A93B-8069635B2A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A33CB5-BC96-4F15-8F16-8752754171FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
   <si>
     <t>Date</t>
   </si>
@@ -188,9 +188,6 @@
   </si>
   <si>
     <t>394, 735, 225, 496</t>
-  </si>
-  <si>
-    <t>need to do 394 and 735 yet</t>
   </si>
 </sst>
 </file>
@@ -613,7 +610,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -905,7 +902,7 @@
         <v>53</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
still one day behind.
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A33CB5-BC96-4F15-8F16-8752754171FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297A5891-8DBA-4D28-9FA8-4BD40B9079F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
+    <workbookView xWindow="-38490" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -188,6 +188,12 @@
   </si>
   <si>
     <t>394, 735, 225, 496</t>
+  </si>
+  <si>
+    <t>933, 649</t>
+  </si>
+  <si>
+    <t>Linked List - LC75</t>
   </si>
 </sst>
 </file>
@@ -610,7 +616,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -913,10 +919,16 @@
         <v>16</v>
       </c>
       <c r="C16" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -924,10 +936,10 @@
         <v>45987</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C17" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -941,7 +953,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1">
         <v>2</v>

</xml_diff>

<commit_message>
starting on linked lists
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297A5891-8DBA-4D28-9FA8-4BD40B9079F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAC8DC1-A127-4CE5-B9D3-393294471673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38490" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9960" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -259,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -277,6 +277,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -615,22 +618,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B13EEB8-513E-4F27-BA22-1B05F2BB10E7}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="30.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="1" customWidth="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.26953125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="69.453125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="30.81640625" style="1"/>
+    <col min="3" max="3" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="69.44140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="30.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -650,7 +653,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>45973</v>
       </c>
@@ -670,7 +673,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45974</v>
       </c>
@@ -690,7 +693,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>45975</v>
       </c>
@@ -707,7 +710,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>45976</v>
       </c>
@@ -719,7 +722,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>45977</v>
       </c>
@@ -739,7 +742,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45978</v>
       </c>
@@ -759,7 +762,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>45979</v>
       </c>
@@ -779,7 +782,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>45980</v>
       </c>
@@ -799,7 +802,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>45981</v>
       </c>
@@ -819,7 +822,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>45981</v>
       </c>
@@ -839,7 +842,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>45982</v>
       </c>
@@ -859,7 +862,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>45983</v>
       </c>
@@ -871,7 +874,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>45984</v>
       </c>
@@ -891,7 +894,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>45985</v>
       </c>
@@ -911,7 +914,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>45986</v>
       </c>
@@ -931,7 +934,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>45987</v>
       </c>
@@ -944,8 +947,14 @@
       <c r="D17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E17" s="7">
+        <v>2062095</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>45988</v>
       </c>
@@ -959,7 +968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>45989</v>
       </c>
@@ -973,7 +982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>45990</v>
       </c>
@@ -985,7 +994,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>45991</v>
       </c>
@@ -999,7 +1008,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>45992</v>
       </c>
@@ -1013,7 +1022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>45993</v>
       </c>
@@ -1027,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>45994</v>
       </c>
@@ -1041,7 +1050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>45995</v>
       </c>
@@ -1055,7 +1064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>45996</v>
       </c>
@@ -1069,7 +1078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>45997</v>
       </c>
@@ -1081,7 +1090,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>45998</v>
       </c>
@@ -1095,7 +1104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>45999</v>
       </c>
@@ -1109,7 +1118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>46000</v>
       </c>
@@ -1123,7 +1132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>46001</v>
       </c>
@@ -1137,7 +1146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>46002</v>
       </c>
@@ -1151,7 +1160,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>46003</v>
       </c>
@@ -1165,7 +1174,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>46004</v>
       </c>
@@ -1177,7 +1186,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>46005</v>
       </c>
@@ -1191,7 +1200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>46006</v>
       </c>
@@ -1205,7 +1214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>46007</v>
       </c>
@@ -1219,7 +1228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>46008</v>
       </c>
@@ -1233,7 +1242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>46009</v>
       </c>
@@ -1247,7 +1256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>46010</v>
       </c>
@@ -1261,7 +1270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>46011</v>
       </c>
@@ -1273,7 +1282,7 @@
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>46012</v>
       </c>
@@ -1287,7 +1296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>46013</v>
       </c>
@@ -1301,7 +1310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>46014</v>
       </c>
@@ -1315,7 +1324,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>46015</v>
       </c>
@@ -1329,7 +1338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>46016</v>
       </c>
@@ -1341,7 +1350,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46017</v>
       </c>
@@ -1351,7 +1360,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>46018</v>
       </c>
@@ -1361,7 +1370,7 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>46019</v>
       </c>
@@ -1371,7 +1380,7 @@
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>46020</v>
       </c>
@@ -1381,7 +1390,7 @@
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>46021</v>
       </c>
@@ -1391,7 +1400,7 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
     </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>46022</v>
       </c>
@@ -1424,16 +1433,16 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="30.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.81640625" style="1"/>
+    <col min="1" max="1" width="30.77734375" style="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="30.81640625" style="1"/>
+    <col min="3" max="3" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="30.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1453,7 +1462,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45658</v>
       </c>
@@ -1465,7 +1474,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45659</v>
       </c>
@@ -1475,7 +1484,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>45660</v>
       </c>
@@ -1485,7 +1494,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>45661</v>
       </c>
@@ -1495,7 +1504,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>45662</v>
       </c>
@@ -1505,7 +1514,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45663</v>
       </c>
@@ -1515,7 +1524,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>45664</v>
       </c>
@@ -1525,7 +1534,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>45665</v>
       </c>
@@ -1535,7 +1544,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>45666</v>
       </c>
@@ -1545,7 +1554,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>45667</v>
       </c>
@@ -1555,7 +1564,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>45668</v>
       </c>
@@ -1569,7 +1578,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>45669</v>
       </c>
@@ -1583,7 +1592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>45670</v>
       </c>
@@ -1597,7 +1606,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>45671</v>
       </c>
@@ -1611,7 +1620,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>45672</v>
       </c>
@@ -1625,7 +1634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>45673</v>
       </c>
@@ -1639,7 +1648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>45674</v>
       </c>
@@ -1651,7 +1660,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>45675</v>
       </c>
@@ -1665,7 +1674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>45676</v>
       </c>
@@ -1679,7 +1688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>45677</v>
       </c>
@@ -1693,7 +1702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>45678</v>
       </c>
@@ -1707,7 +1716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>45679</v>
       </c>
@@ -1721,7 +1730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>45680</v>
       </c>
@@ -1735,7 +1744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>45681</v>
       </c>
@@ -1747,7 +1756,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>45682</v>
       </c>
@@ -1761,7 +1770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>45683</v>
       </c>
@@ -1775,7 +1784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>45684</v>
       </c>
@@ -1783,7 +1792,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>45685</v>
       </c>
@@ -1791,17 +1800,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>45686</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>45687</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>45688</v>
       </c>
@@ -1813,7 +1822,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>45689</v>
       </c>

</xml_diff>

<commit_message>
one binary tree down. one to go.
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10F603B-FA0A-4122-93AB-9DF76DB94F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983C6114-F2CB-4470-9F5B-DF385EC6508C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38490" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -197,6 +197,15 @@
   </si>
   <si>
     <t>328, 2130</t>
+  </si>
+  <si>
+    <t>Binary Tree - DFS - LC75</t>
+  </si>
+  <si>
+    <t>104, 1448</t>
+  </si>
+  <si>
+    <t>Need to do 1448 still</t>
   </si>
 </sst>
 </file>
@@ -621,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B13EEB8-513E-4F27-BA22-1B05F2BB10E7}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -985,13 +994,19 @@
         <v>45989</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="C19" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
two DFS binary trees down. Feeling good about these ones.
Also lightly updated my helper functions for binary tree printing.
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983C6114-F2CB-4470-9F5B-DF385EC6508C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D9EA63-FCF0-4A72-BF5B-D5CE2850FA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38490" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
+    <workbookView xWindow="-33430" yWindow="1930" windowWidth="28800" windowHeight="15370" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -205,7 +205,7 @@
     <t>104, 1448</t>
   </si>
   <si>
-    <t>Need to do 1448 still</t>
+    <t xml:space="preserve">Need to pick a med for tomorrow as well. Stil half a day behind. </t>
   </si>
 </sst>
 </file>
@@ -630,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B13EEB8-513E-4F27-BA22-1B05F2BB10E7}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1006,7 +1006,7 @@
         <v>58</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1026,13 +1026,19 @@
         <v>45991</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="C21" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>872</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1046,7 +1052,7 @@
         <v>2</v>
       </c>
       <c r="D22" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
need to finish 236. It is the last DFS problem.
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vt653f\Documents\Python\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D9EA63-FCF0-4A72-BF5B-D5CE2850FA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924347D4-AED3-452B-A7FB-7F32E690B0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33430" yWindow="1930" windowWidth="28800" windowHeight="15370" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -205,7 +205,13 @@
     <t>104, 1448</t>
   </si>
   <si>
-    <t xml:space="preserve">Need to pick a med for tomorrow as well. Stil half a day behind. </t>
+    <t>872, 437</t>
+  </si>
+  <si>
+    <t>1372, 236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">need to finish 236 yet, started it. </t>
   </si>
 </sst>
 </file>
@@ -630,22 +636,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B13EEB8-513E-4F27-BA22-1B05F2BB10E7}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.1796875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="69.453125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="30.81640625" style="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="69.42578125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="30.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -665,7 +671,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>45973</v>
       </c>
@@ -685,7 +691,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45974</v>
       </c>
@@ -705,7 +711,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45975</v>
       </c>
@@ -725,7 +731,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45976</v>
       </c>
@@ -737,7 +743,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45977</v>
       </c>
@@ -757,7 +763,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45978</v>
       </c>
@@ -777,7 +783,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45979</v>
       </c>
@@ -797,7 +803,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45980</v>
       </c>
@@ -817,7 +823,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45981</v>
       </c>
@@ -837,7 +843,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45981</v>
       </c>
@@ -857,7 +863,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45982</v>
       </c>
@@ -877,7 +883,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45983</v>
       </c>
@@ -889,7 +895,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45984</v>
       </c>
@@ -909,7 +915,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45985</v>
       </c>
@@ -929,7 +935,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45986</v>
       </c>
@@ -949,7 +955,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45987</v>
       </c>
@@ -969,7 +975,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45988</v>
       </c>
@@ -989,7 +995,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45989</v>
       </c>
@@ -1009,7 +1015,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45990</v>
       </c>
@@ -1021,7 +1027,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45991</v>
       </c>
@@ -1034,14 +1040,14 @@
       <c r="D21" s="1">
         <v>1</v>
       </c>
-      <c r="E21" s="1">
-        <v>872</v>
+      <c r="E21" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45992</v>
       </c>
@@ -1049,13 +1055,19 @@
         <v>18</v>
       </c>
       <c r="C22" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D22" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45993</v>
       </c>
@@ -1069,7 +1081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45994</v>
       </c>
@@ -1083,7 +1095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45995</v>
       </c>
@@ -1097,7 +1109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45996</v>
       </c>
@@ -1111,7 +1123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45997</v>
       </c>
@@ -1123,7 +1135,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>45998</v>
       </c>
@@ -1137,7 +1149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>45999</v>
       </c>
@@ -1151,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>46000</v>
       </c>
@@ -1165,7 +1177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>46001</v>
       </c>
@@ -1179,7 +1191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>46002</v>
       </c>
@@ -1193,7 +1205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>46003</v>
       </c>
@@ -1207,7 +1219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>46004</v>
       </c>
@@ -1219,7 +1231,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>46005</v>
       </c>
@@ -1233,7 +1245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>46006</v>
       </c>
@@ -1247,7 +1259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>46007</v>
       </c>
@@ -1261,7 +1273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>46008</v>
       </c>
@@ -1275,7 +1287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>46009</v>
       </c>
@@ -1289,7 +1301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>46010</v>
       </c>
@@ -1303,7 +1315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>46011</v>
       </c>
@@ -1315,7 +1327,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>46012</v>
       </c>
@@ -1329,7 +1341,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>46013</v>
       </c>
@@ -1343,7 +1355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>46014</v>
       </c>
@@ -1357,7 +1369,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>46015</v>
       </c>
@@ -1371,7 +1383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>46016</v>
       </c>
@@ -1383,7 +1395,7 @@
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
     </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46017</v>
       </c>
@@ -1393,7 +1405,7 @@
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>46018</v>
       </c>
@@ -1403,7 +1415,7 @@
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>46019</v>
       </c>
@@ -1413,7 +1425,7 @@
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>46020</v>
       </c>
@@ -1423,7 +1435,7 @@
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
     </row>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>46021</v>
       </c>
@@ -1433,7 +1445,7 @@
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
     </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>46022</v>
       </c>
@@ -1466,16 +1478,16 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.81640625" style="1"/>
+    <col min="1" max="1" width="30.85546875" style="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="30.81640625" style="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="30.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1495,7 +1507,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45658</v>
       </c>
@@ -1507,7 +1519,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45659</v>
       </c>
@@ -1517,7 +1529,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45660</v>
       </c>
@@ -1527,7 +1539,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45661</v>
       </c>
@@ -1537,7 +1549,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45662</v>
       </c>
@@ -1547,7 +1559,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45663</v>
       </c>
@@ -1557,7 +1569,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45664</v>
       </c>
@@ -1567,7 +1579,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45665</v>
       </c>
@@ -1577,7 +1589,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45666</v>
       </c>
@@ -1587,7 +1599,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45667</v>
       </c>
@@ -1597,7 +1609,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45668</v>
       </c>
@@ -1611,7 +1623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45669</v>
       </c>
@@ -1625,7 +1637,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45670</v>
       </c>
@@ -1639,7 +1651,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45671</v>
       </c>
@@ -1653,7 +1665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45672</v>
       </c>
@@ -1667,7 +1679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45673</v>
       </c>
@@ -1681,7 +1693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45674</v>
       </c>
@@ -1693,7 +1705,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45675</v>
       </c>
@@ -1707,7 +1719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45676</v>
       </c>
@@ -1721,7 +1733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45677</v>
       </c>
@@ -1735,7 +1747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45678</v>
       </c>
@@ -1749,7 +1761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45679</v>
       </c>
@@ -1763,7 +1775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45680</v>
       </c>
@@ -1777,7 +1789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45681</v>
       </c>
@@ -1789,7 +1801,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45682</v>
       </c>
@@ -1803,7 +1815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45683</v>
       </c>
@@ -1817,7 +1829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>45684</v>
       </c>
@@ -1825,7 +1837,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>45685</v>
       </c>
@@ -1833,17 +1845,17 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>45686</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>45687</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>45688</v>
       </c>
@@ -1855,7 +1867,7 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>45689</v>
       </c>

</xml_diff>

<commit_message>
wrapped up the BFS problems.
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vt653f\Documents\Python\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78042E9F-195D-4E67-B898-6BD1CA9A753D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A07AF79-4BB7-47A1-B341-E33334C0F37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15345" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Binary Tree - DFS - LC75+</t>
   </si>
   <si>
-    <t>Binary Search Tree - LC75+</t>
-  </si>
-  <si>
     <t>Graphs DFS - LC75+</t>
   </si>
   <si>
@@ -209,6 +206,12 @@
   </si>
   <si>
     <t>1372, 236</t>
+  </si>
+  <si>
+    <t>1161, 102</t>
+  </si>
+  <si>
+    <t>Binary Search Tree - LC75</t>
   </si>
 </sst>
 </file>
@@ -634,21 +637,21 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.1796875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="69.453125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="30.81640625" style="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="69.42578125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="30.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -668,7 +671,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>45973</v>
       </c>
@@ -682,13 +685,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45974</v>
       </c>
@@ -702,13 +705,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45975</v>
       </c>
@@ -722,13 +725,13 @@
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45976</v>
       </c>
@@ -740,7 +743,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45977</v>
       </c>
@@ -754,13 +757,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45978</v>
       </c>
@@ -774,13 +777,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45979</v>
       </c>
@@ -794,13 +797,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45980</v>
       </c>
@@ -814,13 +817,13 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45981</v>
       </c>
@@ -834,13 +837,13 @@
         <v>0</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45981</v>
       </c>
@@ -854,13 +857,13 @@
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45982</v>
       </c>
@@ -874,13 +877,13 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45983</v>
       </c>
@@ -892,7 +895,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45984</v>
       </c>
@@ -906,13 +909,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45985</v>
       </c>
@@ -926,13 +929,13 @@
         <v>2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45986</v>
       </c>
@@ -946,38 +949,38 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45987</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45988</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
@@ -986,33 +989,33 @@
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45989</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45990</v>
       </c>
@@ -1024,12 +1027,12 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45991</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
@@ -1038,13 +1041,13 @@
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45992</v>
       </c>
@@ -1058,13 +1061,13 @@
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45993</v>
       </c>
@@ -1081,10 +1084,10 @@
         <v>199</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45994</v>
       </c>
@@ -1092,32 +1095,38 @@
         <v>17</v>
       </c>
       <c r="C24" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45995</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="C25" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45996</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C26" s="1">
         <v>3</v>
@@ -1126,7 +1135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45997</v>
       </c>
@@ -1138,12 +1147,12 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>45998</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
@@ -1152,12 +1161,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>45999</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C29" s="1">
         <v>3</v>
@@ -1166,12 +1175,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>46000</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C30" s="1">
         <v>3</v>
@@ -1180,12 +1189,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>46001</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C31" s="1">
         <v>3</v>
@@ -1194,12 +1203,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>46002</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C32" s="1">
         <v>2</v>
@@ -1208,12 +1217,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>46003</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C33" s="1">
         <v>2</v>
@@ -1222,7 +1231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>46004</v>
       </c>
@@ -1234,12 +1243,12 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>46005</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C35" s="1">
         <v>3</v>
@@ -1248,12 +1257,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>46006</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36" s="1">
         <v>3</v>
@@ -1262,12 +1271,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>46007</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C37" s="1">
         <v>3</v>
@@ -1276,12 +1285,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>46008</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C38" s="1">
         <v>3</v>
@@ -1290,12 +1299,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>46009</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C39" s="1">
         <v>3</v>
@@ -1304,12 +1313,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>46010</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C40" s="1">
         <v>3</v>
@@ -1318,7 +1327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>46011</v>
       </c>
@@ -1330,12 +1339,12 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>46012</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C42" s="1">
         <v>2</v>
@@ -1344,12 +1353,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>46013</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C43" s="1">
         <v>3</v>
@@ -1358,12 +1367,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>46014</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C44" s="1">
         <v>2</v>
@@ -1372,12 +1381,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>46015</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C45" s="1">
         <v>3</v>
@@ -1386,19 +1395,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>46016</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
     </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46017</v>
       </c>
@@ -1408,7 +1417,7 @@
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>46018</v>
       </c>
@@ -1418,7 +1427,7 @@
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>46019</v>
       </c>
@@ -1428,7 +1437,7 @@
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>46020</v>
       </c>
@@ -1438,7 +1447,7 @@
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
     </row>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>46021</v>
       </c>
@@ -1448,7 +1457,7 @@
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
     </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>46022</v>
       </c>
@@ -1481,16 +1490,16 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.81640625" style="1"/>
+    <col min="1" max="1" width="30.85546875" style="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="30.81640625" style="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="30.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1510,19 +1519,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45658</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45659</v>
       </c>
@@ -1532,7 +1541,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45660</v>
       </c>
@@ -1542,7 +1551,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45661</v>
       </c>
@@ -1552,7 +1561,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45662</v>
       </c>
@@ -1562,7 +1571,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45663</v>
       </c>
@@ -1572,7 +1581,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45664</v>
       </c>
@@ -1582,7 +1591,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45665</v>
       </c>
@@ -1592,7 +1601,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45666</v>
       </c>
@@ -1602,7 +1611,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45667</v>
       </c>
@@ -1612,12 +1621,12 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45668</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -1626,7 +1635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45669</v>
       </c>
@@ -1640,7 +1649,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45670</v>
       </c>
@@ -1654,12 +1663,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45671</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
@@ -1668,12 +1677,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45672</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="1">
         <v>2</v>
@@ -1682,12 +1691,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45673</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="1">
         <v>3</v>
@@ -1696,7 +1705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45674</v>
       </c>
@@ -1708,12 +1717,12 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45675</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1">
         <v>3</v>
@@ -1722,12 +1731,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45676</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="1">
         <v>3</v>
@@ -1736,12 +1745,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45677</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="1">
         <v>3</v>
@@ -1750,12 +1759,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45678</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="1">
         <v>3</v>
@@ -1764,12 +1773,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45679</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="1">
         <v>3</v>
@@ -1778,12 +1787,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45680</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="1">
         <v>3</v>
@@ -1792,7 +1801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45681</v>
       </c>
@@ -1804,12 +1813,12 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45682</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="1">
         <v>3</v>
@@ -1818,12 +1827,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45683</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" s="1">
         <v>3</v>
@@ -1832,33 +1841,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>45684</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>45685</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>45686</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>45687</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>45688</v>
       </c>
@@ -1870,7 +1879,7 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>45689</v>
       </c>

</xml_diff>

<commit_message>
train is arrving. Did one medium graph problem, will do 547 later.
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vt653f\Documents\Python\Leetcode_Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F62926-543E-4171-BCC5-4A2350627515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93B781B-FF4E-4066-975A-B20492E216FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12" yWindow="12" windowWidth="23016" windowHeight="12216" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="64">
   <si>
     <t>Date</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>700, 450</t>
+  </si>
+  <si>
+    <t>High, still need to do one more. 547</t>
   </si>
 </sst>
 </file>
@@ -640,21 +643,21 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="30.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="69.42578125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="30.85546875" style="1"/>
+    <col min="3" max="3" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="69.44140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="30.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -674,7 +677,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>45973</v>
       </c>
@@ -694,7 +697,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45974</v>
       </c>
@@ -714,7 +717,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>45975</v>
       </c>
@@ -734,7 +737,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>45976</v>
       </c>
@@ -746,7 +749,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>45977</v>
       </c>
@@ -766,7 +769,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45978</v>
       </c>
@@ -786,7 +789,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>45979</v>
       </c>
@@ -806,7 +809,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>45980</v>
       </c>
@@ -826,7 +829,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>45981</v>
       </c>
@@ -846,7 +849,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>45981</v>
       </c>
@@ -866,7 +869,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>45982</v>
       </c>
@@ -886,7 +889,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>45983</v>
       </c>
@@ -898,7 +901,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>45984</v>
       </c>
@@ -918,7 +921,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>45985</v>
       </c>
@@ -938,7 +941,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>45986</v>
       </c>
@@ -958,7 +961,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>45987</v>
       </c>
@@ -978,7 +981,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>45988</v>
       </c>
@@ -998,7 +1001,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>45989</v>
       </c>
@@ -1018,7 +1021,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>45990</v>
       </c>
@@ -1030,7 +1033,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>45991</v>
       </c>
@@ -1050,7 +1053,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>45992</v>
       </c>
@@ -1070,7 +1073,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>45993</v>
       </c>
@@ -1090,7 +1093,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>45994</v>
       </c>
@@ -1110,7 +1113,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>45995</v>
       </c>
@@ -1130,7 +1133,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>45996</v>
       </c>
@@ -1138,13 +1141,19 @@
         <v>19</v>
       </c>
       <c r="C26" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1">
+        <v>841</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>45997</v>
       </c>
@@ -1156,7 +1165,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>45998</v>
       </c>
@@ -1170,7 +1179,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>45999</v>
       </c>
@@ -1184,7 +1193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>46000</v>
       </c>
@@ -1198,7 +1207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>46001</v>
       </c>
@@ -1212,7 +1221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>46002</v>
       </c>
@@ -1226,7 +1235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>46003</v>
       </c>
@@ -1240,7 +1249,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>46004</v>
       </c>
@@ -1252,7 +1261,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>46005</v>
       </c>
@@ -1266,7 +1275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>46006</v>
       </c>
@@ -1280,7 +1289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>46007</v>
       </c>
@@ -1294,7 +1303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>46008</v>
       </c>
@@ -1308,7 +1317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>46009</v>
       </c>
@@ -1322,7 +1331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>46010</v>
       </c>
@@ -1336,7 +1345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>46011</v>
       </c>
@@ -1348,7 +1357,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>46012</v>
       </c>
@@ -1362,7 +1371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>46013</v>
       </c>
@@ -1376,7 +1385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>46014</v>
       </c>
@@ -1390,7 +1399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>46015</v>
       </c>
@@ -1404,7 +1413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>46016</v>
       </c>
@@ -1416,7 +1425,7 @@
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
     </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46017</v>
       </c>
@@ -1426,7 +1435,7 @@
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>46018</v>
       </c>
@@ -1436,7 +1445,7 @@
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>46019</v>
       </c>
@@ -1446,7 +1455,7 @@
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>46020</v>
       </c>
@@ -1456,7 +1465,7 @@
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
     </row>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>46021</v>
       </c>
@@ -1466,7 +1475,7 @@
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
     </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>46022</v>
       </c>
@@ -1499,16 +1508,16 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="30.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" style="1"/>
+    <col min="1" max="1" width="30.88671875" style="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="30.85546875" style="1"/>
+    <col min="3" max="3" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="30.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1528,7 +1537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45658</v>
       </c>
@@ -1540,7 +1549,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45659</v>
       </c>
@@ -1550,7 +1559,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>45660</v>
       </c>
@@ -1560,7 +1569,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>45661</v>
       </c>
@@ -1570,7 +1579,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>45662</v>
       </c>
@@ -1580,7 +1589,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45663</v>
       </c>
@@ -1590,7 +1599,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>45664</v>
       </c>
@@ -1600,7 +1609,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>45665</v>
       </c>
@@ -1610,7 +1619,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>45666</v>
       </c>
@@ -1620,7 +1629,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>45667</v>
       </c>
@@ -1630,7 +1639,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>45668</v>
       </c>
@@ -1644,7 +1653,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>45669</v>
       </c>
@@ -1658,7 +1667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>45670</v>
       </c>
@@ -1672,7 +1681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>45671</v>
       </c>
@@ -1686,7 +1695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>45672</v>
       </c>
@@ -1700,7 +1709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>45673</v>
       </c>
@@ -1714,7 +1723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>45674</v>
       </c>
@@ -1726,7 +1735,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>45675</v>
       </c>
@@ -1740,7 +1749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>45676</v>
       </c>
@@ -1754,7 +1763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>45677</v>
       </c>
@@ -1768,7 +1777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>45678</v>
       </c>
@@ -1782,7 +1791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>45679</v>
       </c>
@@ -1796,7 +1805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>45680</v>
       </c>
@@ -1810,7 +1819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>45681</v>
       </c>
@@ -1822,7 +1831,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>45682</v>
       </c>
@@ -1836,7 +1845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>45683</v>
       </c>
@@ -1850,7 +1859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>45684</v>
       </c>
@@ -1858,7 +1867,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>45685</v>
       </c>
@@ -1866,17 +1875,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>45686</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>45687</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>45688</v>
       </c>
@@ -1888,7 +1897,7 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>45689</v>
       </c>

</xml_diff>

<commit_message>
completed 547, need to do some reading on DFS in graphs.
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93B781B-FF4E-4066-975A-B20492E216FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88975A59-DCA8-4202-8694-C1263B8733B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
+    <workbookView xWindow="-33430" yWindow="1930" windowWidth="28800" windowHeight="15370" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="65">
   <si>
     <t>Date</t>
   </si>
@@ -217,7 +217,10 @@
     <t>700, 450</t>
   </si>
   <si>
-    <t>High, still need to do one more. 547</t>
+    <t>High for the first one, low-med for the second one.</t>
+  </si>
+  <si>
+    <t>841, 547</t>
   </si>
 </sst>
 </file>
@@ -643,21 +646,21 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="B27" sqref="B27:F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="30.90625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" style="1" customWidth="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="69.44140625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="30.88671875" style="1"/>
+    <col min="3" max="3" width="12.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.08984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="69.453125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="30.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -677,7 +680,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>45973</v>
       </c>
@@ -697,7 +700,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>45974</v>
       </c>
@@ -717,7 +720,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>45975</v>
       </c>
@@ -737,7 +740,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>45976</v>
       </c>
@@ -749,7 +752,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>45977</v>
       </c>
@@ -769,7 +772,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>45978</v>
       </c>
@@ -789,7 +792,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45979</v>
       </c>
@@ -809,7 +812,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>45980</v>
       </c>
@@ -829,7 +832,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>45981</v>
       </c>
@@ -849,7 +852,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>45981</v>
       </c>
@@ -869,7 +872,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>45982</v>
       </c>
@@ -889,7 +892,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>45983</v>
       </c>
@@ -901,7 +904,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>45984</v>
       </c>
@@ -921,7 +924,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>45985</v>
       </c>
@@ -941,7 +944,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>45986</v>
       </c>
@@ -961,7 +964,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>45987</v>
       </c>
@@ -981,7 +984,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>45988</v>
       </c>
@@ -1001,7 +1004,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>45989</v>
       </c>
@@ -1021,7 +1024,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>45990</v>
       </c>
@@ -1033,7 +1036,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>45991</v>
       </c>
@@ -1053,7 +1056,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>45992</v>
       </c>
@@ -1073,7 +1076,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>45993</v>
       </c>
@@ -1093,7 +1096,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>45994</v>
       </c>
@@ -1113,7 +1116,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>45995</v>
       </c>
@@ -1133,7 +1136,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>45996</v>
       </c>
@@ -1146,14 +1149,14 @@
       <c r="D26" s="1">
         <v>2</v>
       </c>
-      <c r="E26" s="1">
-        <v>841</v>
+      <c r="E26" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>45997</v>
       </c>
@@ -1165,7 +1168,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>45998</v>
       </c>
@@ -1179,7 +1182,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>45999</v>
       </c>
@@ -1193,7 +1196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>46000</v>
       </c>
@@ -1207,7 +1210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>46001</v>
       </c>
@@ -1221,7 +1224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>46002</v>
       </c>
@@ -1235,7 +1238,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>46003</v>
       </c>
@@ -1249,7 +1252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>46004</v>
       </c>
@@ -1261,7 +1264,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>46005</v>
       </c>
@@ -1275,7 +1278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>46006</v>
       </c>
@@ -1289,7 +1292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>46007</v>
       </c>
@@ -1303,7 +1306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>46008</v>
       </c>
@@ -1317,7 +1320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>46009</v>
       </c>
@@ -1331,7 +1334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>46010</v>
       </c>
@@ -1345,7 +1348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>46011</v>
       </c>
@@ -1357,7 +1360,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>46012</v>
       </c>
@@ -1371,7 +1374,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>46013</v>
       </c>
@@ -1385,7 +1388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>46014</v>
       </c>
@@ -1399,7 +1402,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>46015</v>
       </c>
@@ -1413,7 +1416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>46016</v>
       </c>
@@ -1425,7 +1428,7 @@
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
     </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>46017</v>
       </c>
@@ -1435,7 +1438,7 @@
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>46018</v>
       </c>
@@ -1445,7 +1448,7 @@
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>46019</v>
       </c>
@@ -1455,7 +1458,7 @@
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>46020</v>
       </c>
@@ -1465,7 +1468,7 @@
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
     </row>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>46021</v>
       </c>
@@ -1475,7 +1478,7 @@
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
     </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>46022</v>
       </c>
@@ -1508,16 +1511,16 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="30.90625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" style="1"/>
+    <col min="1" max="1" width="30.90625" style="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="30.88671875" style="1"/>
+    <col min="3" max="3" width="12.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="30.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1537,7 +1540,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>45658</v>
       </c>
@@ -1549,7 +1552,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>45659</v>
       </c>
@@ -1559,7 +1562,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>45660</v>
       </c>
@@ -1569,7 +1572,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>45661</v>
       </c>
@@ -1579,7 +1582,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>45662</v>
       </c>
@@ -1589,7 +1592,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>45663</v>
       </c>
@@ -1599,7 +1602,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45664</v>
       </c>
@@ -1609,7 +1612,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>45665</v>
       </c>
@@ -1619,7 +1622,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>45666</v>
       </c>
@@ -1629,7 +1632,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>45667</v>
       </c>
@@ -1639,7 +1642,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>45668</v>
       </c>
@@ -1653,7 +1656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>45669</v>
       </c>
@@ -1667,7 +1670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>45670</v>
       </c>
@@ -1681,7 +1684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>45671</v>
       </c>
@@ -1695,7 +1698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>45672</v>
       </c>
@@ -1709,7 +1712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>45673</v>
       </c>
@@ -1723,7 +1726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>45674</v>
       </c>
@@ -1735,7 +1738,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>45675</v>
       </c>
@@ -1749,7 +1752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>45676</v>
       </c>
@@ -1763,7 +1766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>45677</v>
       </c>
@@ -1777,7 +1780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>45678</v>
       </c>
@@ -1791,7 +1794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>45679</v>
       </c>
@@ -1805,7 +1808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>45680</v>
       </c>
@@ -1819,7 +1822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>45681</v>
       </c>
@@ -1831,7 +1834,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>45682</v>
       </c>
@@ -1845,7 +1848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>45683</v>
       </c>
@@ -1859,7 +1862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>45684</v>
       </c>
@@ -1867,7 +1870,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>45685</v>
       </c>
@@ -1875,17 +1878,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>45686</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>45687</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>45688</v>
       </c>
@@ -1897,7 +1900,7 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>45689</v>
       </c>

</xml_diff>

<commit_message>
updating the study plan.
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88975A59-DCA8-4202-8694-C1263B8733B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43315F0-BC96-4316-93C3-134AD603FA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33430" yWindow="1930" windowWidth="28800" windowHeight="15370" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Binary Tree - DFS - LC75+</t>
   </si>
   <si>
-    <t>Graphs DFS - LC75+</t>
-  </si>
-  <si>
     <t>Graphs BFS - LC75+</t>
   </si>
   <si>
@@ -221,6 +218,12 @@
   </si>
   <si>
     <t>841, 547</t>
+  </si>
+  <si>
+    <t>Graphs DFS - LC75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pushing to tomorrow. I'm tired. </t>
   </si>
 </sst>
 </file>
@@ -645,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B13EEB8-513E-4F27-BA22-1B05F2BB10E7}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:F27"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.90625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -694,10 +697,10 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -714,10 +717,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -734,10 +737,10 @@
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -766,10 +769,10 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -786,10 +789,10 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -806,10 +809,10 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -826,10 +829,10 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -846,10 +849,10 @@
         <v>0</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -866,10 +869,10 @@
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -886,10 +889,10 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -918,10 +921,10 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -938,10 +941,10 @@
         <v>2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -958,10 +961,10 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -969,19 +972,19 @@
         <v>45987</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>54</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -989,7 +992,7 @@
         <v>45988</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
@@ -998,10 +1001,10 @@
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1009,19 +1012,19 @@
         <v>45989</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1041,7 +1044,7 @@
         <v>45991</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
@@ -1050,10 +1053,10 @@
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1070,10 +1073,10 @@
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1093,7 +1096,7 @@
         <v>199</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1110,10 +1113,10 @@
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1121,19 +1124,19 @@
         <v>45995</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="F25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1141,7 +1144,7 @@
         <v>45996</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="C26" s="1">
         <v>0</v>
@@ -1150,10 +1153,10 @@
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1173,13 +1176,16 @@
         <v>45998</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="C28" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D28" s="1">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1187,10 +1193,10 @@
         <v>45999</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="C29" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
@@ -1201,7 +1207,7 @@
         <v>46000</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30" s="1">
         <v>3</v>
@@ -1215,7 +1221,7 @@
         <v>46001</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C31" s="1">
         <v>3</v>
@@ -1229,7 +1235,7 @@
         <v>46002</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C32" s="1">
         <v>2</v>
@@ -1243,7 +1249,7 @@
         <v>46003</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C33" s="1">
         <v>2</v>
@@ -1269,7 +1275,7 @@
         <v>46005</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C35" s="1">
         <v>3</v>
@@ -1283,7 +1289,7 @@
         <v>46006</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C36" s="1">
         <v>3</v>
@@ -1297,7 +1303,7 @@
         <v>46007</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C37" s="1">
         <v>3</v>
@@ -1311,7 +1317,7 @@
         <v>46008</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C38" s="1">
         <v>3</v>
@@ -1325,7 +1331,7 @@
         <v>46009</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C39" s="1">
         <v>3</v>
@@ -1339,7 +1345,7 @@
         <v>46010</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C40" s="1">
         <v>3</v>
@@ -1365,7 +1371,7 @@
         <v>46012</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C42" s="1">
         <v>2</v>
@@ -1379,7 +1385,7 @@
         <v>46013</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C43" s="1">
         <v>3</v>
@@ -1393,7 +1399,7 @@
         <v>46014</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C44" s="1">
         <v>2</v>
@@ -1407,7 +1413,7 @@
         <v>46015</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C45" s="1">
         <v>3</v>
@@ -1421,7 +1427,7 @@
         <v>46016</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
@@ -1545,7 +1551,7 @@
         <v>45658</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -1647,7 +1653,7 @@
         <v>45668</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -1689,7 +1695,7 @@
         <v>45671</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
@@ -1703,7 +1709,7 @@
         <v>45672</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1">
         <v>2</v>
@@ -1717,7 +1723,7 @@
         <v>45673</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="1">
         <v>3</v>
@@ -1743,7 +1749,7 @@
         <v>45675</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" s="1">
         <v>3</v>
@@ -1757,7 +1763,7 @@
         <v>45676</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="1">
         <v>3</v>
@@ -1771,7 +1777,7 @@
         <v>45677</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="1">
         <v>3</v>
@@ -1785,7 +1791,7 @@
         <v>45678</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="1">
         <v>3</v>
@@ -1799,7 +1805,7 @@
         <v>45679</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="1">
         <v>3</v>
@@ -1813,7 +1819,7 @@
         <v>45680</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" s="1">
         <v>3</v>
@@ -1839,7 +1845,7 @@
         <v>45682</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" s="1">
         <v>3</v>
@@ -1853,7 +1859,7 @@
         <v>45683</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" s="1">
         <v>3</v>
@@ -1867,7 +1873,7 @@
         <v>45684</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1875,7 +1881,7 @@
         <v>45685</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
finally got through the graph problem. more tomorrow.
</commit_message>
<xml_diff>
--- a/studyPlan.xlsx
+++ b/studyPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakeg\Documents\Leetcode_Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vt653f\Documents\Python\Leetcode_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43315F0-BC96-4316-93C3-134AD603FA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC45274A-1F2D-4057-A744-F5941AB4764E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33430" yWindow="1930" windowWidth="28800" windowHeight="15370" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{40E157FC-66F1-4DA4-8DA1-715D5785E706}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -223,7 +223,7 @@
     <t>Graphs DFS - LC75</t>
   </si>
   <si>
-    <t xml:space="preserve">Pushing to tomorrow. I'm tired. </t>
+    <t xml:space="preserve">Low-Med. This is a fantastic question to come back to. </t>
   </si>
 </sst>
 </file>
@@ -649,21 +649,21 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.90625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.08984375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="69.453125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="30.90625" style="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="69.42578125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="30.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -683,7 +683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>45973</v>
       </c>
@@ -703,7 +703,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45974</v>
       </c>
@@ -723,7 +723,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45975</v>
       </c>
@@ -743,7 +743,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45976</v>
       </c>
@@ -755,7 +755,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45977</v>
       </c>
@@ -775,7 +775,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45978</v>
       </c>
@@ -795,7 +795,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45979</v>
       </c>
@@ -815,7 +815,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45980</v>
       </c>
@@ -835,7 +835,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45981</v>
       </c>
@@ -855,7 +855,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45981</v>
       </c>
@@ -875,7 +875,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45982</v>
       </c>
@@ -895,7 +895,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45983</v>
       </c>
@@ -907,7 +907,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45984</v>
       </c>
@@ -927,7 +927,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45985</v>
       </c>
@@ -947,7 +947,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45986</v>
       </c>
@@ -967,7 +967,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45987</v>
       </c>
@@ -987,7 +987,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45988</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45989</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45990</v>
       </c>
@@ -1039,7 +1039,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45991</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45992</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45993</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45994</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45995</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45996</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45997</v>
       </c>
@@ -1171,7 +1171,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>45998</v>
       </c>
@@ -1184,11 +1184,14 @@
       <c r="D28" s="1">
         <v>1</v>
       </c>
+      <c r="E28" s="1">
+        <v>1466</v>
+      </c>
       <c r="F28" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>45999</v>
       </c>
@@ -1202,7 +1205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>46000</v>
       </c>
@@ -1216,7 +1219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>46001</v>
       </c>
@@ -1230,7 +1233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>46002</v>
       </c>
@@ -1244,7 +1247,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>46003</v>
       </c>
@@ -1258,7 +1261,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>46004</v>
       </c>
@@ -1270,7 +1273,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>46005</v>
       </c>
@@ -1284,7 +1287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>46006</v>
       </c>
@@ -1298,7 +1301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>46007</v>
       </c>
@@ -1312,7 +1315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>46008</v>
       </c>
@@ -1326,7 +1329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>46009</v>
       </c>
@@ -1340,7 +1343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>46010</v>
       </c>
@@ -1354,7 +1357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>46011</v>
       </c>
@@ -1366,7 +1369,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>46012</v>
       </c>
@@ -1380,7 +1383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>46013</v>
       </c>
@@ -1394,7 +1397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>46014</v>
       </c>
@@ -1408,7 +1411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>46015</v>
       </c>
@@ -1422,7 +1425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>46016</v>
       </c>
@@ -1434,7 +1437,7 @@
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
     </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46017</v>
       </c>
@@ -1444,7 +1447,7 @@
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>46018</v>
       </c>
@@ -1454,7 +1457,7 @@
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>46019</v>
       </c>
@@ -1464,7 +1467,7 @@
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>46020</v>
       </c>
@@ -1474,7 +1477,7 @@
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
     </row>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>46021</v>
       </c>
@@ -1484,7 +1487,7 @@
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
     </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>46022</v>
       </c>
@@ -1517,16 +1520,16 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.90625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.90625" style="1"/>
+    <col min="1" max="1" width="30.85546875" style="1"/>
     <col min="2" max="2" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="30.90625" style="1"/>
+    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="30.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1546,7 +1549,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45658</v>
       </c>
@@ -1558,7 +1561,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45659</v>
       </c>
@@ -1568,7 +1571,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45660</v>
       </c>
@@ -1578,7 +1581,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45661</v>
       </c>
@@ -1588,7 +1591,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45662</v>
       </c>
@@ -1598,7 +1601,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45663</v>
       </c>
@@ -1608,7 +1611,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45664</v>
       </c>
@@ -1618,7 +1621,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45665</v>
       </c>
@@ -1628,7 +1631,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45666</v>
       </c>
@@ -1638,7 +1641,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45667</v>
       </c>
@@ -1648,7 +1651,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45668</v>
       </c>
@@ -1662,7 +1665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45669</v>
       </c>
@@ -1676,7 +1679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45670</v>
       </c>
@@ -1690,7 +1693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45671</v>
       </c>
@@ -1704,7 +1707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45672</v>
       </c>
@@ -1718,7 +1721,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45673</v>
       </c>
@@ -1732,7 +1735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45674</v>
       </c>
@@ -1744,7 +1747,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45675</v>
       </c>
@@ -1758,7 +1761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45676</v>
       </c>
@@ -1772,7 +1775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45677</v>
       </c>
@@ -1786,7 +1789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45678</v>
       </c>
@@ -1800,7 +1803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45679</v>
       </c>
@@ -1814,7 +1817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45680</v>
       </c>
@@ -1828,7 +1831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45681</v>
       </c>
@@ -1840,7 +1843,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45682</v>
       </c>
@@ -1854,7 +1857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45683</v>
       </c>
@@ -1868,7 +1871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>45684</v>
       </c>
@@ -1876,7 +1879,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>45685</v>
       </c>
@@ -1884,17 +1887,17 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>45686</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>45687</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>45688</v>
       </c>
@@ -1906,7 +1909,7 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>45689</v>
       </c>

</xml_diff>